<commit_message>
update choose_category function, add print_last_game function
</commit_message>
<xml_diff>
--- a/Player_db.xlsx
+++ b/Player_db.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit\Desktop\new project\Stark_Industries\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80A1D887-2E7E-4A5F-BD9B-2F09EA7E41DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t>ID</t>
   </si>
@@ -95,20 +101,26 @@
   </si>
   <si>
     <t>Question7</t>
+  </si>
+  <si>
+    <t>Parent_1</t>
+  </si>
+  <si>
+    <t>Parent_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -116,7 +128,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -156,18 +168,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -214,7 +235,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -246,9 +267,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,6 +319,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -455,14 +512,35 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.125" customWidth="1"/>
+    <col min="2" max="2" width="11.125" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="13.375" customWidth="1"/>
+    <col min="5" max="5" width="11" customWidth="1"/>
+    <col min="6" max="6" width="10.5" customWidth="1"/>
+    <col min="7" max="7" width="12.25" customWidth="1"/>
+    <col min="8" max="8" width="10" customWidth="1"/>
+    <col min="9" max="9" width="12.625" customWidth="1"/>
+    <col min="10" max="10" width="10.75" customWidth="1"/>
+    <col min="11" max="11" width="12.625" customWidth="1"/>
+    <col min="12" max="12" width="13" customWidth="1"/>
+    <col min="13" max="13" width="12.875" customWidth="1"/>
+    <col min="14" max="14" width="11.375" customWidth="1"/>
+    <col min="15" max="15" width="12.125" customWidth="1"/>
+    <col min="16" max="16" width="10.125" customWidth="1"/>
+    <col min="17" max="17" width="10.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:15">
+    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -505,8 +583,14 @@
       <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -553,7 +637,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:15">
+    <row r="3" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -600,7 +684,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:15">
+    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -644,7 +728,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:15">
+    <row r="5" spans="1:17" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -654,5 +738,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>